<commit_message>
Correzione report-checklist.xslt caso 78
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#EUROCHIMICASRLXX/EUROCHIMICA/EMAGING-RIS/1.1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#EUROCHIMICASRLXX/EUROCHIMICA/EMAGING-RIS/1.1.0/report-checklist.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="212">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -939,7 +939,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1024,12 +1024,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1164,7 +1158,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1309,11 +1303,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3647,11 +3637,11 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="9" topLeftCell="J26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="9" topLeftCell="K17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
-      <selection pane="bottomRight" activeCell="N26" activeCellId="0" sqref="N26"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="K20" activeCellId="0" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4200,7 +4190,7 @@
       <c r="O16" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="P16" s="36" t="s">
+      <c r="P16" s="31" t="s">
         <v>79</v>
       </c>
       <c r="Q16" s="31"/>
@@ -4285,10 +4275,10 @@
       <c r="L18" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="M18" s="36" t="s">
+      <c r="M18" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="N18" s="36" t="s">
+      <c r="N18" s="31" t="s">
         <v>88</v>
       </c>
       <c r="O18" s="31" t="s">
@@ -4370,18 +4360,22 @@
       <c r="I20" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="J20" s="31"/>
+      <c r="J20" s="31" t="s">
+        <v>55</v>
+      </c>
       <c r="K20" s="31"/>
       <c r="L20" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="M20" s="36" t="s">
+      <c r="M20" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="N20" s="36" t="s">
+      <c r="N20" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="O20" s="31"/>
+      <c r="O20" s="31" t="s">
+        <v>55</v>
+      </c>
       <c r="P20" s="31" t="s">
         <v>89</v>
       </c>
@@ -4620,18 +4614,18 @@
       <c r="M26" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="N26" s="36" t="s">
+      <c r="N26" s="31" t="s">
         <v>119</v>
       </c>
       <c r="O26" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="P26" s="36" t="s">
+      <c r="P26" s="31" t="s">
         <v>120</v>
       </c>
       <c r="Q26" s="31"/>
       <c r="R26" s="32"/>
-      <c r="S26" s="37"/>
+      <c r="S26" s="36"/>
       <c r="T26" s="34" t="s">
         <v>72</v>
       </c>
@@ -4650,12 +4644,12 @@
       <c r="K27" s="31"/>
       <c r="L27" s="31"/>
       <c r="M27" s="31"/>
-      <c r="N27" s="36"/>
+      <c r="N27" s="31"/>
       <c r="O27" s="31"/>
-      <c r="P27" s="36"/>
+      <c r="P27" s="31"/>
       <c r="Q27" s="31"/>
       <c r="R27" s="32"/>
-      <c r="S27" s="37"/>
+      <c r="S27" s="36"/>
       <c r="T27" s="34"/>
     </row>
     <row r="28" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10085,7 +10079,7 @@
   <hyperlinks>
     <hyperlink ref="E10" r:id="rId2" display="&#10;Viene richiamato il servizio di validazione &quot;https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation&quot; al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway&#10;&#10;Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione &quot;CASO DI TEST 1&quot; riportata nei documenti &quot;casi di test RAD&quot; e &quot;CDA2_Referto_di_Radiologia_OK&quot; presenti al path https://github.com/ministero-salute/it-fse-accreditamento."/>
     <hyperlink ref="E11" r:id="rId3" display="&#10;Viene richiamato il servizio di validazione &quot;https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation&quot; al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway&#10;&#10;Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione &quot;CASO DI TEST 2&quot; riportata nei documenti &quot;casi di test RAD&quot; e &quot;CDA2_Referto_di_Radiologia_OK&quot; presenti al path https://github.com/ministero-salute/it-fse-accreditamento."/>
-    <hyperlink ref="E26" r:id="rId4" display="https://github.com/ministero-salute/it-fse-accreditamento"/>
+    <hyperlink ref="E26" r:id="rId4" display="Viene richiamato il servizio di validazione &quot;https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation&quot; al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.&#10; &#10;I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione &quot;CASO DI TEST 14&quot; riportata nei documenti &quot;casi di test RAD&quot; e &quot;CDA2_Referto_di_Radiologia_KO&quot; presenti al path https://github.com/ministero-salute/it-fse-accreditamento."/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -10140,10 +10134,10 @@
       <c r="B2" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="37" t="s">
         <v>157</v>
       </c>
     </row>
@@ -10154,10 +10148,10 @@
       <c r="B3" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="37" t="s">
         <v>160</v>
       </c>
     </row>
@@ -10168,10 +10162,10 @@
       <c r="B4" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="38" t="s">
         <v>162</v>
       </c>
     </row>
@@ -10182,10 +10176,10 @@
       <c r="B5" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="37" t="s">
         <v>165</v>
       </c>
     </row>
@@ -10196,10 +10190,10 @@
       <c r="B6" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="38" t="s">
         <v>168</v>
       </c>
     </row>
@@ -10210,10 +10204,10 @@
       <c r="B7" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="38" t="s">
         <v>171</v>
       </c>
     </row>
@@ -10224,10 +10218,10 @@
       <c r="B8" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="38" t="s">
         <v>174</v>
       </c>
     </row>
@@ -10238,10 +10232,10 @@
       <c r="B9" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="38" t="s">
         <v>177</v>
       </c>
     </row>
@@ -10252,10 +10246,10 @@
       <c r="B10" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="37" t="s">
         <v>180</v>
       </c>
     </row>
@@ -10266,10 +10260,10 @@
       <c r="B11" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C11" s="38" t="n">
+      <c r="C11" s="37" t="n">
         <v>192</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="37" t="s">
         <v>182</v>
       </c>
     </row>
@@ -10280,10 +10274,10 @@
       <c r="B12" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C12" s="38" t="n">
+      <c r="C12" s="37" t="n">
         <v>208</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="37" t="s">
         <v>183</v>
       </c>
     </row>
@@ -10294,10 +10288,10 @@
       <c r="B13" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C13" s="38" t="n">
+      <c r="C13" s="37" t="n">
         <v>224</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="38" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10308,10 +10302,10 @@
       <c r="B14" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C14" s="38" t="n">
+      <c r="C14" s="37" t="n">
         <v>240</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="37" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10322,10 +10316,10 @@
       <c r="B15" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C15" s="38" t="n">
+      <c r="C15" s="37" t="n">
         <v>256</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="38" t="s">
         <v>186</v>
       </c>
     </row>
@@ -10336,10 +10330,10 @@
       <c r="B16" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C16" s="38" t="n">
+      <c r="C16" s="37" t="n">
         <v>272</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="38" t="s">
         <v>187</v>
       </c>
     </row>
@@ -10350,10 +10344,10 @@
       <c r="B17" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C17" s="38" t="n">
+      <c r="C17" s="37" t="n">
         <v>288</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="38" t="s">
         <v>188</v>
       </c>
     </row>
@@ -10364,10 +10358,10 @@
       <c r="B18" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C18" s="38" t="n">
+      <c r="C18" s="37" t="n">
         <v>304</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="38" t="s">
         <v>189</v>
       </c>
     </row>
@@ -10378,10 +10372,10 @@
       <c r="B19" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="C19" s="38" t="n">
+      <c r="C19" s="37" t="n">
         <v>193</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="37" t="s">
         <v>191</v>
       </c>
     </row>
@@ -10392,10 +10386,10 @@
       <c r="B20" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="C20" s="38" t="n">
+      <c r="C20" s="37" t="n">
         <v>209</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="37" t="s">
         <v>192</v>
       </c>
     </row>
@@ -10406,10 +10400,10 @@
       <c r="B21" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="C21" s="38" t="n">
+      <c r="C21" s="37" t="n">
         <v>225</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="38" t="s">
         <v>193</v>
       </c>
     </row>
@@ -10420,10 +10414,10 @@
       <c r="B22" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="C22" s="38" t="n">
+      <c r="C22" s="37" t="n">
         <v>241</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="37" t="s">
         <v>194</v>
       </c>
     </row>
@@ -10434,10 +10428,10 @@
       <c r="B23" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="C23" s="38" t="n">
+      <c r="C23" s="37" t="n">
         <v>257</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="38" t="s">
         <v>195</v>
       </c>
     </row>
@@ -10448,10 +10442,10 @@
       <c r="B24" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="C24" s="38" t="n">
+      <c r="C24" s="37" t="n">
         <v>273</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="38" t="s">
         <v>196</v>
       </c>
     </row>
@@ -10462,10 +10456,10 @@
       <c r="B25" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="C25" s="38" t="n">
+      <c r="C25" s="37" t="n">
         <v>289</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="D25" s="38" t="s">
         <v>197</v>
       </c>
     </row>
@@ -10476,10 +10470,10 @@
       <c r="B26" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="C26" s="38" t="n">
+      <c r="C26" s="37" t="n">
         <v>305</v>
       </c>
-      <c r="D26" s="39" t="s">
+      <c r="D26" s="38" t="s">
         <v>198</v>
       </c>
     </row>
@@ -10490,10 +10484,10 @@
       <c r="B27" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="C27" s="38" t="n">
+      <c r="C27" s="37" t="n">
         <v>194</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="37" t="s">
         <v>200</v>
       </c>
     </row>
@@ -10504,10 +10498,10 @@
       <c r="B28" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="C28" s="38" t="n">
+      <c r="C28" s="37" t="n">
         <v>210</v>
       </c>
-      <c r="D28" s="38" t="s">
+      <c r="D28" s="37" t="s">
         <v>201</v>
       </c>
     </row>
@@ -10518,10 +10512,10 @@
       <c r="B29" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="C29" s="38" t="n">
+      <c r="C29" s="37" t="n">
         <v>226</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="39" t="s">
         <v>202</v>
       </c>
     </row>
@@ -10532,10 +10526,10 @@
       <c r="B30" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="C30" s="38" t="n">
+      <c r="C30" s="37" t="n">
         <v>242</v>
       </c>
-      <c r="D30" s="38" t="s">
+      <c r="D30" s="37" t="s">
         <v>203</v>
       </c>
     </row>
@@ -10546,10 +10540,10 @@
       <c r="B31" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="C31" s="38" t="n">
+      <c r="C31" s="37" t="n">
         <v>258</v>
       </c>
-      <c r="D31" s="39" t="s">
+      <c r="D31" s="38" t="s">
         <v>204</v>
       </c>
     </row>
@@ -10560,10 +10554,10 @@
       <c r="B32" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="C32" s="38" t="n">
+      <c r="C32" s="37" t="n">
         <v>274</v>
       </c>
-      <c r="D32" s="39" t="s">
+      <c r="D32" s="38" t="s">
         <v>205</v>
       </c>
     </row>
@@ -10574,10 +10568,10 @@
       <c r="B33" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="C33" s="38" t="n">
+      <c r="C33" s="37" t="n">
         <v>290</v>
       </c>
-      <c r="D33" s="39" t="s">
+      <c r="D33" s="38" t="s">
         <v>206</v>
       </c>
     </row>
@@ -10588,10 +10582,10 @@
       <c r="B34" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="C34" s="38" t="n">
+      <c r="C34" s="37" t="n">
         <v>306</v>
       </c>
-      <c r="D34" s="39" t="s">
+      <c r="D34" s="38" t="s">
         <v>207</v>
       </c>
     </row>
@@ -10602,10 +10596,10 @@
       <c r="B35" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C35" s="38" t="n">
+      <c r="C35" s="37" t="n">
         <v>195</v>
       </c>
-      <c r="D35" s="38" t="n">
+      <c r="D35" s="37" t="n">
         <v>204</v>
       </c>
     </row>
@@ -10616,10 +10610,10 @@
       <c r="B36" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C36" s="38" t="n">
+      <c r="C36" s="37" t="n">
         <v>211</v>
       </c>
-      <c r="D36" s="38" t="n">
+      <c r="D36" s="37" t="n">
         <v>220</v>
       </c>
     </row>
@@ -10630,10 +10624,10 @@
       <c r="B37" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C37" s="38" t="n">
+      <c r="C37" s="37" t="n">
         <v>227</v>
       </c>
-      <c r="D37" s="39" t="n">
+      <c r="D37" s="38" t="n">
         <v>236</v>
       </c>
     </row>
@@ -10644,10 +10638,10 @@
       <c r="B38" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C38" s="38" t="n">
+      <c r="C38" s="37" t="n">
         <v>243</v>
       </c>
-      <c r="D38" s="38" t="n">
+      <c r="D38" s="37" t="n">
         <v>252</v>
       </c>
     </row>
@@ -10658,10 +10652,10 @@
       <c r="B39" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C39" s="38" t="n">
+      <c r="C39" s="37" t="n">
         <v>259</v>
       </c>
-      <c r="D39" s="39" t="n">
+      <c r="D39" s="38" t="n">
         <v>268</v>
       </c>
     </row>
@@ -10672,10 +10666,10 @@
       <c r="B40" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C40" s="38" t="n">
+      <c r="C40" s="37" t="n">
         <v>275</v>
       </c>
-      <c r="D40" s="39" t="n">
+      <c r="D40" s="38" t="n">
         <v>284</v>
       </c>
     </row>
@@ -10686,10 +10680,10 @@
       <c r="B41" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C41" s="38" t="n">
+      <c r="C41" s="37" t="n">
         <v>291</v>
       </c>
-      <c r="D41" s="39" t="n">
+      <c r="D41" s="38" t="n">
         <v>300</v>
       </c>
     </row>
@@ -10700,10 +10694,10 @@
       <c r="B42" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C42" s="38" t="n">
+      <c r="C42" s="37" t="n">
         <v>307</v>
       </c>
-      <c r="D42" s="39" t="n">
+      <c r="D42" s="38" t="n">
         <v>316</v>
       </c>
     </row>
@@ -10714,10 +10708,10 @@
       <c r="B43" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="C43" s="38" t="n">
+      <c r="C43" s="37" t="n">
         <v>196</v>
       </c>
-      <c r="D43" s="38" t="n">
+      <c r="D43" s="37" t="n">
         <v>207</v>
       </c>
     </row>
@@ -10728,10 +10722,10 @@
       <c r="B44" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="C44" s="38" t="n">
+      <c r="C44" s="37" t="n">
         <v>212</v>
       </c>
-      <c r="D44" s="38" t="n">
+      <c r="D44" s="37" t="n">
         <v>223</v>
       </c>
     </row>
@@ -10742,10 +10736,10 @@
       <c r="B45" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="C45" s="38" t="n">
+      <c r="C45" s="37" t="n">
         <v>228</v>
       </c>
-      <c r="D45" s="39" t="n">
+      <c r="D45" s="38" t="n">
         <v>239</v>
       </c>
     </row>
@@ -10756,10 +10750,10 @@
       <c r="B46" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="C46" s="38" t="n">
+      <c r="C46" s="37" t="n">
         <v>244</v>
       </c>
-      <c r="D46" s="38" t="n">
+      <c r="D46" s="37" t="n">
         <v>255</v>
       </c>
     </row>
@@ -10770,10 +10764,10 @@
       <c r="B47" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="C47" s="38" t="n">
+      <c r="C47" s="37" t="n">
         <v>260</v>
       </c>
-      <c r="D47" s="39" t="n">
+      <c r="D47" s="38" t="n">
         <v>271</v>
       </c>
     </row>
@@ -10784,10 +10778,10 @@
       <c r="B48" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="C48" s="38" t="n">
+      <c r="C48" s="37" t="n">
         <v>276</v>
       </c>
-      <c r="D48" s="39" t="n">
+      <c r="D48" s="38" t="n">
         <v>287</v>
       </c>
     </row>
@@ -10798,10 +10792,10 @@
       <c r="B49" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="C49" s="38" t="n">
+      <c r="C49" s="37" t="n">
         <v>292</v>
       </c>
-      <c r="D49" s="39" t="n">
+      <c r="D49" s="38" t="n">
         <v>303</v>
       </c>
     </row>
@@ -10812,10 +10806,10 @@
       <c r="B50" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="C50" s="38" t="n">
+      <c r="C50" s="37" t="n">
         <v>308</v>
       </c>
-      <c r="D50" s="39" t="n">
+      <c r="D50" s="38" t="n">
         <v>319</v>
       </c>
     </row>
@@ -11799,32 +11793,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="40" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="40" t="s">
         <v>211</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="40" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Replica Test case 11
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#EUROCHIMICASRLXX/EUROCHIMICA/EMAGING-RIS/1.1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#EUROCHIMICASRLXX/EUROCHIMICA/EMAGING-RIS/1.1.0/report-checklist.xlsx
@@ -293,13 +293,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-06-12T10:58:10Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24f2c36f1dd58c01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.190.4.4.9803f00db507e677d24e947483aa0286ec83c1eb184d6cd68a11105d8e25cdf7.8c40a95532^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-06-21T08:46:10Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a666ad2cfab94bab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.190.4.4.a8dd3226aa77e3065e6aaeb7083002ca765c67d363def609447b6ec27522045d.b683abca76^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">SI</t>
@@ -632,7 +632,7 @@
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.190.4.4.2774d04d9c7cd592979593e26cb23fa0a7c12f16b8547768e571313bfedd214c.d66bd535d1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t xml:space="preserve">Errore di sintassi</t>
+    <t xml:space="preserve">ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'text'. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id, \"urn:hl7-org:v3\":code}' is expected.</t>
   </si>
   <si>
     <t xml:space="preserve">Il cliente non è autonomo nel compiere l’assegnazione dei codici ICD-9-CM o LOINC alle proprie prestazioni.
@@ -3637,11 +3637,11 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="9" topLeftCell="K17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="K20" activeCellId="0" sqref="K20"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3894,7 +3894,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="25" t="n">
         <v>11</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>51</v>
       </c>
       <c r="F10" s="28" t="n">
-        <v>45455</v>
+        <v>45464</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Replica Test case 84
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#EUROCHIMICASRLXX/EUROCHIMICA/EMAGING-RIS/1.1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#EUROCHIMICASRLXX/EUROCHIMICA/EMAGING-RIS/1.1.0/report-checklist.xlsx
@@ -623,13 +623,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-06-17T13:26:05Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e2e8fc51252997b8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.190.4.4.2774d04d9c7cd592979593e26cb23fa0a7c12f16b8547768e571313bfedd214c.d66bd535d1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-06-21T09:12:09Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4d35c8eb1a689be9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.190.4.4.7f8e2a3dfef2d3119ff9bd027b362af751f4178cd214d98651cde0102e39bc7e.245a4f25ac^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'text'. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id, \"urn:hl7-org:v3\":code}' is expected.</t>
@@ -3637,11 +3637,11 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="9" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="I26" activeCellId="0" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4593,7 +4593,7 @@
         <v>115</v>
       </c>
       <c r="F26" s="28" t="n">
-        <v>45460</v>
+        <v>45464</v>
       </c>
       <c r="G26" s="29" t="s">
         <v>116</v>

</xml_diff>